<commit_message>
bug fixes, scd 2
</commit_message>
<xml_diff>
--- a/AzureDWHFramework/AzureDWHFrameworkDataInput/DataInput.xlsx
+++ b/AzureDWHFramework/AzureDWHFrameworkDataInput/DataInput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\source\repos\AzureDWHframework\AzureDWHFramework\AzureDWHFrameworkDataInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\source\repos\AzureDWHFramework\AzureDWHFramework\AzureDWHFrameworkDataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275A2F4F-BA20-4531-A923-B61391681B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4F9028-7EAD-49FA-A42C-FD963D5C3EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Business Area" sheetId="12" r:id="rId1"/>
@@ -57,9 +57,9 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A97A3F6D-258A-47C2-A556-02F0EA8396ED}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t xml:space="preserve">[Komentář ve vlákně]
+Vaše verze aplikace Excel vám umožňuje číst tento komentář ve vlákně, ale jakékoli jeho úpravy se odeberou, pokud se soubor otevře v novější verzi aplikace Excel. Další informace: https://go.microsoft.com/fwlink/?linkid=870924
+Komentář:
     SCD1 or SCD2
 </t>
       </text>
@@ -76,9 +76,9 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{F6EABC82-789E-47F4-973F-9396278280B8}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Komentář ve vlákně]
+Vaše verze aplikace Excel vám umožňuje číst tento komentář ve vlákně, ale jakékoli jeho úpravy se odeberou, pokud se soubor otevře v novější verzi aplikace Excel. Další informace: https://go.microsoft.com/fwlink/?linkid=870924
+Komentář:
     Full or Increment</t>
       </text>
     </comment>
@@ -95,17 +95,17 @@
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B7616948-429F-462A-BE7D-FEF744E778FA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Komentář ve vlákně]
+Vaše verze aplikace Excel vám umožňuje číst tento komentář ve vlákně, ale jakékoli jeho úpravy se odeberou, pokud se soubor otevře v novější verzi aplikace Excel. Další informace: https://go.microsoft.com/fwlink/?linkid=870924
+Komentář:
     Leave blank when column is not referencing to dimension</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1" shapeId="0" xr:uid="{322A949E-A72E-425E-8252-7370C9F16B86}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Komentář ve vlákně]
+Vaše verze aplikace Excel vám umožňuje číst tento komentář ve vlákně, ale jakékoli jeho úpravy se odeberou, pokud se soubor otevře v novější verzi aplikace Excel. Další informace: https://go.microsoft.com/fwlink/?linkid=870924
+Komentář:
     Leave blank when column is not referencing to dimension</t>
       </text>
     </comment>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="172">
   <si>
     <t>SchemaName</t>
   </si>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>SalesPersonCode</t>
+  </si>
+  <si>
+    <t>EmployeeCode</t>
   </si>
 </sst>
 </file>
@@ -721,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1122,7 +1125,7 @@
   <dimension ref="A1:J3797"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1265,7 @@
   <dimension ref="A1:H4472"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D14"/>
+      <selection activeCell="D6" sqref="D6:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,8 +4181,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4243,8 +4246,8 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4427,21 +4430,168 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
       <c r="L6" t="str">
         <f t="shared" ref="L6:L8" si="0">_xlfn.CONCAT("INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",B6,"' AND SchemaName = N'",A6,"')",",N'",C6, "',N'",J6, "',N'",G6, "',",H6,",",I6,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F6,"' AND stgTable.SchemaName = N'",D6,"' AND stgTable.TableName = N'",E6,"'))")</f>
-        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'' AND SchemaName = N''),N'',N'',N'',,, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'' AND stgTable.SchemaName = N'' AND stgTable.TableName = N''))</v>
+        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'SalesPerson' AND SchemaName = N'dwh'),N'EmployeeCode',N'',N'int',0,1, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'BusinessEntityID' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'Employee'))</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
       <c r="L7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'' AND SchemaName = N''),N'',N'',N'',,, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'' AND stgTable.SchemaName = N'' AND stgTable.TableName = N''))</v>
+        <f t="shared" ref="L7:L10" si="1">_xlfn.CONCAT("INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",B7,"' AND SchemaName = N'",A7,"')",",N'",C7, "',N'",J7, "',N'",G7, "',",H7,",",I7,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F7,"' AND stgTable.SchemaName = N'",D7,"' AND stgTable.TableName = N'",E7,"'))")</f>
+        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'SalesPerson' AND SchemaName = N'dwh'),N'LoginID',N'',N'nvarchar(256)',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'LoginID' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'Employee'))</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
       <c r="L8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'' AND SchemaName = N''),N'',N'',N'',,, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'' AND stgTable.SchemaName = N'' AND stgTable.TableName = N''))</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'SalesPerson' AND SchemaName = N'dwh'),N'JobTitle',N'',N'nvarchar(50)',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'JobTitle' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'Employee'))</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'SalesPerson' AND SchemaName = N'dwh'),N'Gender',N'',N'nchar(1)',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'Gender' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'Employee'))</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.DimensionTableColumn(DimensionTableID, ColumnName,Description, DataType, Nullable, BusinessKey, StageTableColumnID) VALUES ( (SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'SalesPerson' AND SchemaName = N'dwh'),N'MaritalStatus',N'',N'nchar(1)',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'MaritalStatus' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'Employee'))</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -5644,12 +5794,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5818,15 +5965,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF01738-4FB6-4420-ACD5-05F4ADA23550}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C35E53F-2B8C-4469-8C9B-1A3659EAE88B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5851,10 +6002,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C35E53F-2B8C-4469-8C9B-1A3659EAE88B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF01738-4FB6-4420-ACD5-05F4ADA23550}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
sample dwh objects added
</commit_message>
<xml_diff>
--- a/AzureDWHFramework/AzureDWHFrameworkDataInput/DataInput.xlsx
+++ b/AzureDWHFramework/AzureDWHFrameworkDataInput/DataInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\source\repos\AzureDWHframework\AzureDWHFramework\AzureDWHFrameworkDataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475390E8-DF07-4831-B0A2-07955EEC2946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA99ADB2-0FA4-4DF0-99F8-9089C4F979D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Business Area" sheetId="15" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="114">
   <si>
     <t>SchemaName</t>
   </si>
@@ -950,16 +950,16 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H2:H5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H5" si="0" xml:space="preserve"> IF(C4 = "Dimension",_xlfn.CONCAT("INSERT INTO etl.DwhMapping(LoadingProcedureName, DimensionTableID, FactTableID, Active,Layer) VALUES (N'",D4,"',(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",B4,"' AND SchemaName = N'",A4,"')",", NULL,",E4, ",",F4, ")"),_xlfn.CONCAT("INSERT INTO etl.DwhMapping(LoadingProcedureName, FactTableID, DimensionTableID, Active,Layer) VALUES (N'",D4,"',(SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B4,"' AND SchemaName = N'",A4,"')",", NULL,",E4, ",",F4, ")"))</f>
+        <f t="shared" ref="H4:H6" si="0" xml:space="preserve"> IF(C4 = "Dimension",_xlfn.CONCAT("INSERT INTO etl.DwhMapping(LoadingProcedureName, DimensionTableID, FactTableID, Active,Layer) VALUES (N'",D4,"',(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",B4,"' AND SchemaName = N'",A4,"')",", NULL,",E4, ",",F4, ")"),_xlfn.CONCAT("INSERT INTO etl.DwhMapping(LoadingProcedureName, FactTableID, DimensionTableID, Active,Layer) VALUES (N'",D4,"',(SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B4,"' AND SchemaName = N'",A4,"')",", NULL,",E4, ",",F4, ")"))</f>
         <v>INSERT INTO etl.DwhMapping(LoadingProcedureName, DimensionTableID, FactTableID, Active,Layer) VALUES (N'dwh.p_Load_D_Employee',(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'Employee' AND SchemaName = N'dwh'), NULL,1,1)</v>
       </c>
     </row>
@@ -1088,6 +1088,31 @@
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO etl.DwhMapping(LoadingProcedureName, DimensionTableID, FactTableID, Active,Layer) VALUES (N'dwh.p_Load_D_Address',(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'Address' AND SchemaName = N'dwh'), NULL,1,1)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.CONCAT(A6,".p_Load_",IF(C6="Dimension","D_","F_"),B6)</f>
+        <v>dwh.p_Load_F_PurchaseOrderHeader</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO etl.DwhMapping(LoadingProcedureName, FactTableID, DimensionTableID, Active,Layer) VALUES (N'dwh.p_Load_F_PurchaseOrderHeader',(SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'), NULL,1,1)</v>
       </c>
     </row>
   </sheetData>
@@ -1099,7 +1124,7 @@
           <x14:formula1>
             <xm:f>HiddenSheet!$C$6:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5</xm:sqref>
+          <xm:sqref>C2:C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1145,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4924,10 +4949,10 @@
   <sheetPr codeName="Sheet8">
     <tabColor rgb="FF70AD47"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4992,6 +5017,27 @@
         <v>INSERT INTO conf.FactTable(SchemaName, TableName, LoadType,BusinessAreas,TabularModels, DeleteCondition, IncrementCondition, LoadWithIncrement) VALUES (N'dwh',N'SalesOrderHeader',N'Full',N'Sales',N'',N'',N'',N'0')</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("INSERT INTO conf.FactTable(SchemaName, TableName, LoadType,BusinessAreas,TabularModels, DeleteCondition, IncrementCondition, LoadWithIncrement) VALUES (N'",A3,"',N'",B3,"',N'",C3,"',N'",D3,"',N'",E3,"',N'",F3,"',N'",G3,"',N'",H3,"')")</f>
+        <v>INSERT INTO conf.FactTable(SchemaName, TableName, LoadType,BusinessAreas,TabularModels, DeleteCondition, IncrementCondition, LoadWithIncrement) VALUES (N'dwh',N'PurchaseOrderHeader',N'Full',N'Purchasing',N'',N'',N'',N'0')</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5003,11 +5049,11 @@
   <sheetPr codeName="Sheet9">
     <tabColor rgb="FF70AD47"/>
   </sheetPr>
-  <dimension ref="A1:O95"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5458,11 +5504,290 @@
         <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'SalesOrderHeader' AND SchemaName = N'dwh'),N'Freight',N'money',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'Freight' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'SalesOrderHeader'),NULL,NULL)</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" s="6"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" s="6"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="str">
+        <f>IF(ISBLANK(G12),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B12,"' AND SchemaName = N'",A12,"')",",N'",C12, "',N'",I12, "',",J12,",",K12,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F12,"' AND stgTable.SchemaName = N'",D12,"' AND stgTable.TableName = N'",E12,"'),","NULL,","NULL)"),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B12,"' AND SchemaName = N'",A12,"')",",N'",C12, "',N'",I12, "',",J12,",",K12,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F12,"' AND stgTable.SchemaName = N'",D12,"' AND stgTable.TableName = N'",E12,"'),","(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",H12,"' AND SchemaName = N'",G12,"'),",J12,")"))</f>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'SalesOrderID',N'int',0,1, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'PurchaseOrderID' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" ref="O13:O19" si="1">IF(ISBLANK(G13),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B13,"' AND SchemaName = N'",A13,"')",",N'",C13, "',N'",I13, "',",J13,",",K13,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F13,"' AND stgTable.SchemaName = N'",D13,"' AND stgTable.TableName = N'",E13,"'),","NULL,","NULL)"),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B13,"' AND SchemaName = N'",A13,"')",",N'",C13, "',N'",I13, "',",J13,",",K13,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F13,"' AND stgTable.SchemaName = N'",D13,"' AND stgTable.TableName = N'",E13,"'),","(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",H13,"' AND SchemaName = N'",G13,"'),",J13,")"))</f>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'SalesPersonID',N'int',1,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'EmployeeID' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'Employee' AND SchemaName = N'dwh'),1)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'ShipDateID',N'int',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'ShipDate' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'Date' AND SchemaName = N'dwh'),0)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'OrderDateID',N'int',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'OrderDate' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'Date' AND SchemaName = N'dwh'),0)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'SubTotal',N'money',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'SubTotal' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'TaxAmt',N'money',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'TaxAmt' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'PurchaseOrderHeader' AND SchemaName = N'dwh'),N'Freight',N'money',0,0, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'Freight' AND stgTable.SchemaName = N'stage_onpremisedb' AND stgTable.TableName = N'PurchaseOrderHeader'),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'' AND SchemaName = N''),N'',N'',,, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'' AND stgTable.SchemaName = N'' AND stgTable.TableName = N''),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O20" t="str">
+        <f>IF(ISBLANK(G20),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B20,"' AND SchemaName = N'",A20,"')",",N'",C20, "',N'",I20, "',",J20,",",K20,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F20,"' AND stgTable.SchemaName = N'",D20,"' AND stgTable.TableName = N'",E20,"'),","NULL,","NULL)"),_xlfn.CONCAT("INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'",B20,"' AND SchemaName = N'",A20,"')",",N'",C20, "',N'",I20, "',",J20,",",K20,", (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'",F20,"' AND stgTable.SchemaName = N'",D20,"' AND stgTable.TableName = N'",E20,"'),","(SELECT DimensionTableID FROM conf.DimensionTable WHERE TableName = N'",H20,"' AND SchemaName = N'",G20,"'),",J20,")"))</f>
+        <v>INSERT INTO conf.FactTableColumn(FactTableID, ColumnName, DataType, Nullable, BusinessKey, StageTableColumnID, DimensionTableID, MainRelationship) VALUES ( (SELECT FactTableID FROM conf.FactTable WHERE TableName = N'' AND SchemaName = N''),N'',N'',,, (SELECT stgColumn.StageTableColumnID FROM conf.StageTable stgTable INNER JOIN conf.StageTableColumn stgColumn ON stgColumn.StageTableID = stgTable.StageTableID WHERE stgColumn.ColumnName = N'' AND stgTable.SchemaName = N'' AND stgTable.TableName = N''),NULL,NULL)</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="6"/>
@@ -5470,8 +5795,8 @@
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="6"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="7"/>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="6"/>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
@@ -5484,6 +5809,9 @@
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5493,9 +5821,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5664,19 +5995,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C35E53F-2B8C-4469-8C9B-1A3659EAE88B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF01738-4FB6-4420-ACD5-05F4ADA23550}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5701,9 +6028,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF01738-4FB6-4420-ACD5-05F4ADA23550}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C35E53F-2B8C-4469-8C9B-1A3659EAE88B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>